<commit_message>
updated ID in spreadsheet (using only upper case)
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/LandMark/LMM-PICL.xlsx
+++ b/Simple_XLS_Importer/data/LandMark/LMM-PICL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\LandMark\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -415,13 +415,13 @@
     <t>All data entries labelled with "no data" were excluded</t>
   </si>
   <si>
-    <t>PICL-2fr</t>
-  </si>
-  <si>
-    <t>PICL-3nfr</t>
-  </si>
-  <si>
-    <t>PICL-1tot</t>
+    <t>PICL-2FR</t>
+  </si>
+  <si>
+    <t>PICL-3NFR</t>
+  </si>
+  <si>
+    <t>PICL-1TOT</t>
   </si>
 </sst>
 </file>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -867,7 +867,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>16</v>
@@ -876,693 +876,693 @@
         <v>2015</v>
       </c>
       <c r="D2" s="7">
-        <v>0</v>
+        <v>76.900000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5">
         <v>2015</v>
       </c>
       <c r="D3" s="7">
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" s="5">
         <v>2015</v>
       </c>
       <c r="D4" s="7">
-        <v>0</v>
+        <v>74.099999999999994</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5">
         <v>2015</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C6" s="5">
         <v>2015</v>
       </c>
       <c r="D6" s="7">
-        <v>0</v>
+        <v>77.900000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5">
         <v>2015</v>
       </c>
       <c r="D7" s="7">
-        <v>0</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5">
         <v>2015</v>
       </c>
       <c r="D8" s="7">
-        <v>0</v>
+        <v>31.6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5">
         <v>2015</v>
       </c>
       <c r="D9" s="7">
-        <v>0</v>
+        <v>71.3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5">
         <v>2015</v>
       </c>
       <c r="D10" s="7">
-        <v>0</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5">
         <v>2015</v>
       </c>
       <c r="D11" s="7">
-        <v>0</v>
+        <v>74.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5">
         <v>2015</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>82.2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5">
         <v>2015</v>
       </c>
       <c r="D13" s="7">
-        <v>0</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="C14" s="5">
         <v>2015</v>
       </c>
       <c r="D14" s="7">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C15" s="5">
         <v>2015</v>
       </c>
       <c r="D15" s="7">
-        <v>0</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C16" s="5">
         <v>2015</v>
       </c>
       <c r="D16" s="7">
-        <v>0</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C17" s="5">
         <v>2015</v>
       </c>
       <c r="D17" s="7">
-        <v>0</v>
+        <v>92.1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5">
         <v>2015</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C19" s="5">
         <v>2015</v>
       </c>
       <c r="D19" s="7">
-        <v>0</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="C20" s="5">
         <v>2015</v>
       </c>
       <c r="D20" s="7">
-        <v>0</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="C21" s="5">
         <v>2015</v>
       </c>
       <c r="D21" s="7">
-        <v>0</v>
+        <v>93.3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="C22" s="5">
         <v>2015</v>
       </c>
       <c r="D22" s="7">
-        <v>0</v>
+        <v>81.099999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="C23" s="5">
         <v>2015</v>
       </c>
       <c r="D23" s="7">
-        <v>0</v>
+        <v>82.9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C24" s="5">
         <v>2015</v>
       </c>
       <c r="D24" s="7">
-        <v>0</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="C25" s="5">
         <v>2015</v>
       </c>
       <c r="D25" s="7">
-        <v>0</v>
+        <v>92.2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C26" s="5">
         <v>2015</v>
       </c>
       <c r="D26" s="7">
-        <v>0</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C27" s="5">
         <v>2015</v>
       </c>
       <c r="D27" s="7">
-        <v>0</v>
+        <v>61.6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="C28" s="5">
         <v>2015</v>
       </c>
       <c r="D28" s="7">
-        <v>0</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C29" s="5">
         <v>2015</v>
       </c>
       <c r="D29" s="7">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5">
         <v>2015</v>
       </c>
       <c r="D30" s="7">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="C31" s="5">
         <v>2015</v>
       </c>
       <c r="D31" s="7">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="C32" s="5">
         <v>2015</v>
       </c>
       <c r="D32" s="7">
-        <v>0</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5">
         <v>2015</v>
       </c>
       <c r="D33" s="7">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="C34" s="5">
         <v>2015</v>
       </c>
       <c r="D34" s="7">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="C35" s="5">
         <v>2015</v>
       </c>
       <c r="D35" s="7">
-        <v>0</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5">
         <v>2015</v>
       </c>
       <c r="D36" s="7">
-        <v>0</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C37" s="5">
         <v>2015</v>
       </c>
       <c r="D37" s="7">
-        <v>0</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="C38" s="5">
         <v>2015</v>
       </c>
       <c r="D38" s="7">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="C39" s="5">
         <v>2015</v>
       </c>
       <c r="D39" s="7">
-        <v>0</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="C40" s="5">
         <v>2015</v>
       </c>
       <c r="D40" s="7">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C41" s="5">
         <v>2015</v>
       </c>
       <c r="D41" s="7">
-        <v>0</v>
+        <v>96.4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5">
         <v>2015</v>
       </c>
       <c r="D42" s="7">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="C43" s="5">
         <v>2015</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="C44" s="5">
         <v>2015</v>
       </c>
       <c r="D44" s="7">
-        <v>0.04</v>
+        <v>81.8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="C45" s="5">
         <v>2015</v>
       </c>
       <c r="D45" s="7">
-        <v>0.1</v>
+        <v>82.3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C46" s="5">
         <v>2015</v>
       </c>
       <c r="D46" s="7">
-        <v>0.1</v>
+        <v>47.9</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C47" s="5">
         <v>2015</v>
       </c>
       <c r="D47" s="7">
-        <v>0.1</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="C48" s="5">
         <v>2015</v>
       </c>
       <c r="D48" s="7">
-        <v>0.5</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="C49" s="5">
         <v>2015</v>
       </c>
       <c r="D49" s="7">
-        <v>0.5</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C50" s="5">
         <v>2015</v>
       </c>
       <c r="D50" s="7">
-        <v>0.9</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C51" s="5">
         <v>2015</v>
       </c>
       <c r="D51" s="7">
-        <v>1.4</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1570,130 +1570,130 @@
         <v>130</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C52" s="5">
         <v>2015</v>
       </c>
       <c r="D52" s="7">
-        <v>2.2000000000000002</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C53" s="5">
         <v>2015</v>
       </c>
       <c r="D53" s="7">
-        <v>2.2000000000000002</v>
+        <v>95.4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C54" s="5">
         <v>2015</v>
       </c>
       <c r="D54" s="7">
-        <v>2.2999999999999998</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="C55" s="5">
         <v>2015</v>
       </c>
       <c r="D55" s="7">
-        <v>2.6</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C56" s="5">
         <v>2015</v>
       </c>
       <c r="D56" s="7">
-        <v>2.9</v>
+        <v>88.9</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="C57" s="5">
         <v>2015</v>
       </c>
       <c r="D57" s="7">
-        <v>3.1</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C58" s="5">
         <v>2015</v>
       </c>
       <c r="D58" s="7">
-        <v>3.2</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C59" s="5">
         <v>2015</v>
       </c>
       <c r="D59" s="7">
-        <v>3.2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="C60" s="5">
         <v>2015</v>
       </c>
       <c r="D60" s="7">
-        <v>3.3</v>
+        <v>68.7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>118</v>
@@ -1702,49 +1702,49 @@
         <v>2015</v>
       </c>
       <c r="D61" s="7">
-        <v>3.7</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="C62" s="5">
         <v>2015</v>
       </c>
       <c r="D62" s="7">
-        <v>4.4000000000000004</v>
+        <v>25.9</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="C63" s="5">
         <v>2015</v>
       </c>
       <c r="D63" s="7">
-        <v>4.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C64" s="5">
         <v>2015</v>
       </c>
       <c r="D64" s="7">
-        <v>5</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,13 +1752,13 @@
         <v>130</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="C65" s="5">
         <v>2015</v>
       </c>
       <c r="D65" s="7">
-        <v>5.5</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1766,13 +1766,13 @@
         <v>128</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="C66" s="5">
         <v>2015</v>
       </c>
       <c r="D66" s="7">
-        <v>5.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1780,27 +1780,27 @@
         <v>128</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C67" s="5">
         <v>2015</v>
       </c>
       <c r="D67" s="7">
-        <v>6.4</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>118</v>
+        <v>17</v>
       </c>
       <c r="C68" s="5">
         <v>2015</v>
       </c>
       <c r="D68" s="7">
-        <v>6.8</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1808,27 +1808,27 @@
         <v>128</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C69" s="5">
         <v>2015</v>
       </c>
       <c r="D69" s="7">
-        <v>7.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="C70" s="5">
         <v>2015</v>
       </c>
       <c r="D70" s="7">
-        <v>7.9</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1836,13 +1836,13 @@
         <v>128</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C71" s="5">
         <v>2015</v>
       </c>
       <c r="D71" s="7">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1850,27 +1850,27 @@
         <v>128</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C72" s="5">
         <v>2015</v>
       </c>
       <c r="D72" s="7">
-        <v>8.6999999999999993</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C73" s="5">
         <v>2015</v>
       </c>
       <c r="D73" s="7">
-        <v>9.1999999999999993</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1878,13 +1878,13 @@
         <v>128</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C74" s="5">
         <v>2015</v>
       </c>
       <c r="D74" s="7">
-        <v>9.3000000000000007</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1892,41 +1892,41 @@
         <v>128</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C75" s="5">
         <v>2015</v>
       </c>
       <c r="D75" s="7">
-        <v>10</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C76" s="5">
         <v>2015</v>
       </c>
       <c r="D76" s="7">
-        <v>11</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="C77" s="5">
         <v>2015</v>
       </c>
       <c r="D77" s="7">
-        <v>11.5</v>
+        <v>71.3</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1934,13 +1934,13 @@
         <v>128</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C78" s="5">
         <v>2015</v>
       </c>
       <c r="D78" s="7">
-        <v>11.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1948,27 +1948,27 @@
         <v>128</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C79" s="5">
         <v>2015</v>
       </c>
       <c r="D79" s="7">
-        <v>11.9</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C80" s="5">
         <v>2015</v>
       </c>
       <c r="D80" s="7">
-        <v>13</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1976,13 +1976,13 @@
         <v>128</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="C81" s="5">
         <v>2015</v>
       </c>
       <c r="D81" s="7">
-        <v>13</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1990,13 +1990,13 @@
         <v>128</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="C82" s="5">
         <v>2015</v>
       </c>
       <c r="D82" s="7">
-        <v>13.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2004,13 +2004,13 @@
         <v>128</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C83" s="5">
         <v>2015</v>
       </c>
       <c r="D83" s="7">
-        <v>14</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2018,13 +2018,13 @@
         <v>128</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C84" s="5">
         <v>2015</v>
       </c>
       <c r="D84" s="7">
-        <v>14.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2032,13 +2032,13 @@
         <v>128</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C85" s="5">
         <v>2015</v>
       </c>
       <c r="D85" s="7">
-        <v>14.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2046,13 +2046,13 @@
         <v>128</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C86" s="5">
         <v>2015</v>
       </c>
       <c r="D86" s="7">
-        <v>14.7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2060,13 +2060,13 @@
         <v>128</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C87" s="5">
         <v>2015</v>
       </c>
       <c r="D87" s="7">
-        <v>15.3</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2074,13 +2074,13 @@
         <v>128</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C88" s="5">
         <v>2015</v>
       </c>
       <c r="D88" s="7">
-        <v>16.600000000000001</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2088,13 +2088,13 @@
         <v>128</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C89" s="5">
         <v>2015</v>
       </c>
       <c r="D89" s="7">
-        <v>16.7</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2102,27 +2102,27 @@
         <v>128</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C90" s="5">
         <v>2015</v>
       </c>
       <c r="D90" s="7">
-        <v>17.3</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C91" s="5">
         <v>2015</v>
       </c>
       <c r="D91" s="7">
-        <v>19.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2130,13 +2130,13 @@
         <v>128</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C92" s="5">
         <v>2015</v>
       </c>
       <c r="D92" s="7">
-        <v>19.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2144,27 +2144,27 @@
         <v>128</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="C93" s="5">
         <v>2015</v>
       </c>
       <c r="D93" s="7">
-        <v>19.600000000000001</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C94" s="5">
         <v>2015</v>
       </c>
       <c r="D94" s="7">
-        <v>20.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2172,13 +2172,13 @@
         <v>128</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C95" s="5">
         <v>2015</v>
       </c>
       <c r="D95" s="7">
-        <v>21.3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2186,55 +2186,55 @@
         <v>128</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="C96" s="5">
         <v>2015</v>
       </c>
       <c r="D96" s="7">
-        <v>22.4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C97" s="5">
         <v>2015</v>
       </c>
       <c r="D97" s="7">
-        <v>22.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="C98" s="5">
         <v>2015</v>
       </c>
       <c r="D98" s="7">
-        <v>22.7</v>
+        <v>79.599999999999994</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C99" s="5">
         <v>2015</v>
       </c>
       <c r="D99" s="7">
-        <v>23</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2242,27 +2242,27 @@
         <v>128</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C100" s="5">
         <v>2015</v>
       </c>
       <c r="D100" s="7">
-        <v>23.3</v>
+        <v>86.5</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>121</v>
+        <v>42</v>
       </c>
       <c r="C101" s="5">
         <v>2015</v>
       </c>
       <c r="D101" s="7">
-        <v>25.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2270,55 +2270,55 @@
         <v>128</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="C102" s="5">
         <v>2015</v>
       </c>
       <c r="D102" s="7">
-        <v>27.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C103" s="5">
         <v>2015</v>
       </c>
       <c r="D103" s="7">
-        <v>28.3</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C104" s="5">
         <v>2015</v>
       </c>
       <c r="D104" s="7">
-        <v>30.6</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C105" s="5">
         <v>2015</v>
       </c>
       <c r="D105" s="7">
-        <v>31.6</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2326,13 +2326,13 @@
         <v>128</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C106" s="5">
         <v>2015</v>
       </c>
       <c r="D106" s="7">
-        <v>31.7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2340,13 +2340,13 @@
         <v>128</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C107" s="5">
         <v>2015</v>
       </c>
       <c r="D107" s="7">
-        <v>32.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2354,27 +2354,27 @@
         <v>128</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C108" s="5">
         <v>2015</v>
       </c>
       <c r="D108" s="7">
-        <v>33.9</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C109" s="5">
         <v>2015</v>
       </c>
       <c r="D109" s="7">
-        <v>34.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2382,27 +2382,27 @@
         <v>128</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="C110" s="5">
         <v>2015</v>
       </c>
       <c r="D110" s="7">
-        <v>34.9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C111" s="5">
         <v>2015</v>
       </c>
       <c r="D111" s="7">
-        <v>36</v>
+        <v>40.1</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2410,27 +2410,27 @@
         <v>128</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="C112" s="5">
         <v>2015</v>
       </c>
       <c r="D112" s="7">
-        <v>36</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C113" s="5">
         <v>2015</v>
       </c>
       <c r="D113" s="7">
-        <v>36.299999999999997</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -2438,13 +2438,13 @@
         <v>128</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C114" s="5">
         <v>2015</v>
       </c>
       <c r="D114" s="7">
-        <v>36.299999999999997</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2452,13 +2452,13 @@
         <v>128</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C115" s="5">
         <v>2015</v>
       </c>
       <c r="D115" s="7">
-        <v>36.4</v>
+        <v>31.7</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2466,41 +2466,41 @@
         <v>128</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C116" s="5">
         <v>2015</v>
       </c>
       <c r="D116" s="7">
-        <v>40.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="C117" s="5">
         <v>2015</v>
       </c>
       <c r="D117" s="7">
-        <v>41.6</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="C118" s="5">
         <v>2015</v>
       </c>
       <c r="D118" s="7">
-        <v>42.4</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2508,13 +2508,13 @@
         <v>128</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="C119" s="5">
         <v>2015</v>
       </c>
       <c r="D119" s="7">
-        <v>42.4</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2522,13 +2522,13 @@
         <v>128</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C120" s="5">
         <v>2015</v>
       </c>
       <c r="D120" s="7">
-        <v>44.1</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2536,27 +2536,27 @@
         <v>128</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C121" s="5">
         <v>2015</v>
       </c>
       <c r="D121" s="7">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C122" s="5">
         <v>2015</v>
       </c>
       <c r="D122" s="7">
-        <v>47.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2564,27 +2564,27 @@
         <v>128</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C123" s="5">
         <v>2015</v>
       </c>
       <c r="D123" s="7">
-        <v>49.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="C124" s="5">
         <v>2015</v>
       </c>
       <c r="D124" s="7">
-        <v>54</v>
+        <v>67.400000000000006</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2592,13 +2592,13 @@
         <v>128</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="C125" s="5">
         <v>2015</v>
       </c>
       <c r="D125" s="7">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2606,27 +2606,27 @@
         <v>128</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C126" s="5">
         <v>2015</v>
       </c>
       <c r="D126" s="7">
-        <v>55.6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C127" s="5">
         <v>2015</v>
       </c>
       <c r="D127" s="7">
-        <v>55.6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2634,41 +2634,41 @@
         <v>128</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C128" s="5">
         <v>2015</v>
       </c>
       <c r="D128" s="7">
-        <v>58</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C129" s="5">
         <v>2015</v>
       </c>
       <c r="D129" s="7">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C130" s="5">
         <v>2015</v>
       </c>
       <c r="D130" s="7">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2676,69 +2676,69 @@
         <v>128</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C131" s="5">
         <v>2015</v>
       </c>
       <c r="D131" s="7">
-        <v>60</v>
+        <v>82.3</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C132" s="5">
         <v>2015</v>
       </c>
       <c r="D132" s="7">
-        <v>60</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="C133" s="5">
         <v>2015</v>
       </c>
       <c r="D133" s="7">
-        <v>61.2</v>
+        <v>98.5</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="C134" s="5">
         <v>2015</v>
       </c>
       <c r="D134" s="7">
-        <v>61.6</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C135" s="5">
         <v>2015</v>
       </c>
       <c r="D135" s="7">
-        <v>64.099999999999994</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -2746,13 +2746,13 @@
         <v>128</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="C136" s="5">
         <v>2015</v>
       </c>
       <c r="D136" s="7">
-        <v>64.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2760,27 +2760,27 @@
         <v>128</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C137" s="5">
         <v>2015</v>
       </c>
       <c r="D137" s="7">
-        <v>65</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C138" s="5">
         <v>2015</v>
       </c>
       <c r="D138" s="7">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -2788,27 +2788,27 @@
         <v>128</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="C139" s="5">
         <v>2015</v>
       </c>
       <c r="D139" s="7">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C140" s="5">
         <v>2015</v>
       </c>
       <c r="D140" s="7">
-        <v>66.400000000000006</v>
+        <v>34.9</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -2816,27 +2816,27 @@
         <v>128</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C141" s="5">
         <v>2015</v>
       </c>
       <c r="D141" s="7">
-        <v>67.400000000000006</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C142" s="5">
         <v>2015</v>
       </c>
       <c r="D142" s="7">
-        <v>67.5</v>
+        <v>97</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -2844,27 +2844,27 @@
         <v>128</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C143" s="5">
         <v>2015</v>
       </c>
       <c r="D143" s="7">
-        <v>67.5</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C144" s="5">
         <v>2015</v>
       </c>
       <c r="D144" s="7">
-        <v>68.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -2872,41 +2872,41 @@
         <v>128</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C145" s="5">
         <v>2015</v>
       </c>
       <c r="D145" s="7">
-        <v>68.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C146" s="5">
         <v>2015</v>
       </c>
       <c r="D146" s="7">
-        <v>69.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C147" s="5">
         <v>2015</v>
       </c>
       <c r="D147" s="7">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -2914,55 +2914,55 @@
         <v>128</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C148" s="5">
         <v>2015</v>
       </c>
       <c r="D148" s="7">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>42</v>
+        <v>101</v>
       </c>
       <c r="C149" s="5">
         <v>2015</v>
       </c>
       <c r="D149" s="7">
-        <v>70.8</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C150" s="5">
         <v>2015</v>
       </c>
       <c r="D150" s="7">
-        <v>70.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="C151" s="5">
         <v>2015</v>
       </c>
       <c r="D151" s="7">
-        <v>71.3</v>
+        <v>95.4</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -2970,153 +2970,153 @@
         <v>128</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="C152" s="5">
         <v>2015</v>
       </c>
       <c r="D152" s="7">
-        <v>71.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C153" s="5">
         <v>2015</v>
       </c>
       <c r="D153" s="7">
-        <v>71.8</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C154" s="5">
         <v>2015</v>
       </c>
       <c r="D154" s="7">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C155" s="5">
         <v>2015</v>
       </c>
       <c r="D155" s="7">
-        <v>73.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C156" s="5">
         <v>2015</v>
       </c>
       <c r="D156" s="7">
-        <v>73.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="C157" s="5">
         <v>2015</v>
       </c>
       <c r="D157" s="7">
-        <v>74.099999999999994</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="C158" s="5">
         <v>2015</v>
       </c>
       <c r="D158" s="7">
-        <v>74.400000000000006</v>
+        <v>98</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C159" s="5">
         <v>2015</v>
       </c>
       <c r="D159" s="7">
-        <v>74.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="C160" s="5">
         <v>2015</v>
       </c>
       <c r="D160" s="7">
-        <v>76</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C161" s="5">
         <v>2015</v>
       </c>
       <c r="D161" s="7">
-        <v>76.8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C162" s="5">
         <v>2015</v>
       </c>
       <c r="D162" s="7">
-        <v>76.8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3124,69 +3124,69 @@
         <v>128</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C163" s="5">
         <v>2015</v>
       </c>
       <c r="D163" s="7">
-        <v>76.8</v>
+        <v>68.7</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="C164" s="5">
         <v>2015</v>
       </c>
       <c r="D164" s="7">
-        <v>76.900000000000006</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C165" s="5">
         <v>2015</v>
       </c>
       <c r="D165" s="7">
-        <v>77.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="C166" s="5">
         <v>2015</v>
       </c>
       <c r="D166" s="7">
-        <v>77.900000000000006</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C167" s="5">
         <v>2015</v>
       </c>
       <c r="D167" s="7">
-        <v>79.599999999999994</v>
+        <v>98</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -3194,13 +3194,13 @@
         <v>128</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C168" s="5">
         <v>2015</v>
       </c>
       <c r="D168" s="7">
-        <v>79.599999999999994</v>
+        <v>81</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3208,55 +3208,55 @@
         <v>128</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C169" s="5">
         <v>2015</v>
       </c>
       <c r="D169" s="7">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C170" s="5">
         <v>2015</v>
       </c>
       <c r="D170" s="7">
-        <v>81.099999999999994</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="C171" s="5">
         <v>2015</v>
       </c>
       <c r="D171" s="7">
-        <v>81.8</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C172" s="5">
         <v>2015</v>
       </c>
       <c r="D172" s="7">
-        <v>81.900000000000006</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -3264,69 +3264,69 @@
         <v>129</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C173" s="5">
         <v>2015</v>
       </c>
       <c r="D173" s="7">
-        <v>81.900000000000006</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C174" s="5">
         <v>2015</v>
       </c>
       <c r="D174" s="7">
-        <v>82.2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="C175" s="5">
         <v>2015</v>
       </c>
       <c r="D175" s="7">
-        <v>82.3</v>
+        <v>41.6</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C176" s="5">
         <v>2015</v>
       </c>
       <c r="D176" s="7">
-        <v>82.3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C177" s="5">
         <v>2015</v>
       </c>
       <c r="D177" s="7">
-        <v>82.9</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -3334,13 +3334,13 @@
         <v>129</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C178" s="5">
         <v>2015</v>
       </c>
       <c r="D178" s="7">
-        <v>82.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -3348,27 +3348,27 @@
         <v>129</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C179" s="5">
         <v>2015</v>
       </c>
       <c r="D179" s="7">
-        <v>82.9</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>112</v>
+        <v>22</v>
       </c>
       <c r="C180" s="5">
         <v>2015</v>
       </c>
       <c r="D180" s="7">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3376,69 +3376,69 @@
         <v>129</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="C181" s="5">
         <v>2015</v>
       </c>
       <c r="D181" s="7">
-        <v>83</v>
+        <v>81.900000000000006</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C182" s="5">
         <v>2015</v>
       </c>
       <c r="D182" s="7">
-        <v>83.3</v>
+        <v>74.400000000000006</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C183" s="5">
         <v>2015</v>
       </c>
       <c r="D183" s="7">
-        <v>83.3</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C184" s="5">
         <v>2015</v>
       </c>
       <c r="D184" s="7">
-        <v>85</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C185" s="5">
         <v>2015</v>
       </c>
       <c r="D185" s="7">
-        <v>85.3</v>
+        <v>85.6</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -3446,13 +3446,13 @@
         <v>129</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C186" s="5">
         <v>2015</v>
       </c>
       <c r="D186" s="7">
-        <v>85.3</v>
+        <v>77.8</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -3460,27 +3460,27 @@
         <v>129</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C187" s="5">
         <v>2015</v>
       </c>
       <c r="D187" s="7">
-        <v>85.6</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C188" s="5">
         <v>2015</v>
       </c>
       <c r="D188" s="7">
-        <v>86.4</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.3">
@@ -3488,97 +3488,97 @@
         <v>129</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C189" s="5">
         <v>2015</v>
       </c>
       <c r="D189" s="7">
-        <v>86.4</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C190" s="5">
         <v>2015</v>
       </c>
       <c r="D190" s="7">
-        <v>86.5</v>
+        <v>66.400000000000006</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C191" s="5">
         <v>2015</v>
       </c>
       <c r="D191" s="7">
-        <v>86.5</v>
+        <v>82.9</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C192" s="5">
         <v>2015</v>
       </c>
       <c r="D192" s="7">
-        <v>86.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="C193" s="5">
         <v>2015</v>
       </c>
       <c r="D193" s="7">
-        <v>87</v>
+        <v>82.9</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C194" s="5">
         <v>2015</v>
       </c>
       <c r="D194" s="7">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="C195" s="5">
         <v>2015</v>
       </c>
       <c r="D195" s="7">
-        <v>87.5</v>
+        <v>70.8</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.3">
@@ -3586,41 +3586,41 @@
         <v>129</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C196" s="5">
         <v>2015</v>
       </c>
       <c r="D196" s="7">
-        <v>87.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C197" s="5">
         <v>2015</v>
       </c>
       <c r="D197" s="7">
-        <v>88</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C198" s="5">
         <v>2015</v>
       </c>
       <c r="D198" s="7">
-        <v>88.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
@@ -3628,27 +3628,27 @@
         <v>129</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C199" s="5">
         <v>2015</v>
       </c>
       <c r="D199" s="7">
-        <v>88.9</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C200" s="5">
         <v>2015</v>
       </c>
       <c r="D200" s="7">
-        <v>89.1</v>
+        <v>97.9</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.3">
@@ -3656,27 +3656,27 @@
         <v>129</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C201" s="5">
         <v>2015</v>
       </c>
       <c r="D201" s="7">
-        <v>89.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C202" s="5">
         <v>2015</v>
       </c>
       <c r="D202" s="7">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -3684,55 +3684,55 @@
         <v>129</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C203" s="5">
         <v>2015</v>
       </c>
       <c r="D203" s="7">
-        <v>91.4</v>
+        <v>64.099999999999994</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="C204" s="5">
         <v>2015</v>
       </c>
       <c r="D204" s="7">
-        <v>91.4</v>
+        <v>89.1</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="C205" s="5">
         <v>2015</v>
       </c>
       <c r="D205" s="7">
-        <v>91.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C206" s="5">
         <v>2015</v>
       </c>
       <c r="D206" s="7">
-        <v>91.5</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.3">
@@ -3740,55 +3740,55 @@
         <v>129</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C207" s="5">
         <v>2015</v>
       </c>
       <c r="D207" s="7">
-        <v>91.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C208" s="5">
         <v>2015</v>
       </c>
       <c r="D208" s="7">
-        <v>92.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="C209" s="5">
         <v>2015</v>
       </c>
       <c r="D209" s="7">
-        <v>92.2</v>
+        <v>71.8</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C210" s="5">
         <v>2015</v>
       </c>
       <c r="D210" s="7">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
@@ -3796,153 +3796,153 @@
         <v>129</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="C211" s="5">
         <v>2015</v>
       </c>
       <c r="D211" s="7">
-        <v>93</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="C212" s="5">
         <v>2015</v>
       </c>
       <c r="D212" s="7">
-        <v>93</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="C213" s="5">
         <v>2015</v>
       </c>
       <c r="D213" s="7">
-        <v>93.3</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="C214" s="5">
         <v>2015</v>
       </c>
       <c r="D214" s="7">
-        <v>95</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C215" s="5">
         <v>2015</v>
       </c>
       <c r="D215" s="7">
-        <v>95</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C216" s="5">
         <v>2015</v>
       </c>
       <c r="D216" s="7">
-        <v>95.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C217" s="5">
         <v>2015</v>
       </c>
       <c r="D217" s="7">
-        <v>95.4</v>
+        <v>97.7</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C218" s="5">
         <v>2015</v>
       </c>
       <c r="D218" s="7">
-        <v>96.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C219" s="5">
         <v>2015</v>
       </c>
       <c r="D219" s="7">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C220" s="5">
         <v>2015</v>
       </c>
       <c r="D220" s="7">
-        <v>97.3</v>
+        <v>88.9</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C221" s="5">
         <v>2015</v>
       </c>
       <c r="D221" s="7">
-        <v>97.7</v>
+        <v>83</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
@@ -3950,27 +3950,27 @@
         <v>129</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="C222" s="5">
         <v>2015</v>
       </c>
       <c r="D222" s="7">
-        <v>97.7</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="C223" s="5">
         <v>2015</v>
       </c>
       <c r="D223" s="7">
-        <v>97.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
@@ -3978,88 +3978,88 @@
         <v>129</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="C224" s="5">
         <v>2015</v>
       </c>
       <c r="D224" s="7">
-        <v>97.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C225" s="5">
         <v>2015</v>
       </c>
       <c r="D225" s="7">
-        <v>98</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C226" s="5">
         <v>2015</v>
       </c>
       <c r="D226" s="7">
-        <v>98</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C227" s="5">
         <v>2015</v>
       </c>
       <c r="D227" s="7">
-        <v>98.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="C228" s="5">
         <v>2015</v>
       </c>
       <c r="D228" s="7">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="C229" s="5">
         <v>2015</v>
       </c>
       <c r="D229" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:E229">
-    <sortCondition ref="D2:D229"/>
+    <sortCondition ref="A2:A229"/>
     <sortCondition ref="B2:B229"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>